<commit_message>
Clean commit after removing API key
</commit_message>
<xml_diff>
--- a/EmbeddingScripts/Product Dummy Data.xlsx
+++ b/EmbeddingScripts/Product Dummy Data.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="118">
   <si>
     <t>id</t>
   </si>
@@ -361,18 +361,9 @@
     <t>yellow</t>
   </si>
   <si>
-    <t>pink</t>
-  </si>
-  <si>
-    <t>purple</t>
-  </si>
-  <si>
     <t>blue</t>
   </si>
   <si>
-    <t>orange</t>
-  </si>
-  <si>
     <t>green</t>
   </si>
   <si>
@@ -389,6 +380,18 @@
   </si>
   <si>
     <t>xxlarge</t>
+  </si>
+  <si>
+    <t>mustard</t>
+  </si>
+  <si>
+    <t>dark green</t>
+  </si>
+  <si>
+    <t>navy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">black </t>
   </si>
 </sst>
 </file>
@@ -762,12 +765,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
+    <col min="1" max="1" width="39.19921875" customWidth="1"/>
     <col min="5" max="5" width="23.5" customWidth="1"/>
     <col min="10" max="10" width="14.8984375" customWidth="1"/>
     <col min="11" max="11" width="34.796875" customWidth="1"/>
@@ -890,10 +894,10 @@
         <v>35</v>
       </c>
       <c r="P2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="Q2" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="U2" t="s">
         <v>36</v>
@@ -946,10 +950,10 @@
         <v>35</v>
       </c>
       <c r="P3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="Q3" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="U3" t="s">
         <v>36</v>
@@ -1002,10 +1006,10 @@
         <v>48</v>
       </c>
       <c r="P4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="Q4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="U4" t="s">
         <v>49</v>
@@ -1058,10 +1062,10 @@
         <v>54</v>
       </c>
       <c r="P5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="Q5" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="U5" t="s">
         <v>49</v>
@@ -1114,10 +1118,10 @@
         <v>58</v>
       </c>
       <c r="P6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="Q6" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="U6" t="s">
         <v>49</v>
@@ -1170,10 +1174,10 @@
         <v>48</v>
       </c>
       <c r="P7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="Q7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="U7" t="s">
         <v>49</v>
@@ -1226,7 +1230,7 @@
         <v>65</v>
       </c>
       <c r="P8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="Q8" t="s">
         <v>103</v>
@@ -1282,10 +1286,10 @@
         <v>69</v>
       </c>
       <c r="P9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q9" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="U9" t="s">
         <v>36</v>
@@ -1338,10 +1342,10 @@
         <v>48</v>
       </c>
       <c r="P10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="U10" t="s">
         <v>49</v>
@@ -1394,7 +1398,7 @@
         <v>54</v>
       </c>
       <c r="P11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q11" t="s">
         <v>107</v>
@@ -1450,10 +1454,10 @@
         <v>76</v>
       </c>
       <c r="P12" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U12" t="s">
         <v>49</v>
@@ -1506,10 +1510,10 @@
         <v>76</v>
       </c>
       <c r="P13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U13" t="s">
         <v>49</v>
@@ -1562,10 +1566,10 @@
         <v>48</v>
       </c>
       <c r="P14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="Q14" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="U14" t="s">
         <v>49</v>
@@ -1618,10 +1622,10 @@
         <v>76</v>
       </c>
       <c r="P15" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="Q15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="U15" t="s">
         <v>49</v>
@@ -1674,10 +1678,10 @@
         <v>54</v>
       </c>
       <c r="P16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="Q16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="U16" t="s">
         <v>49</v>
@@ -1730,10 +1734,10 @@
         <v>58</v>
       </c>
       <c r="P17" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="Q17" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="U17" t="s">
         <v>49</v>
@@ -1786,10 +1790,10 @@
         <v>88</v>
       </c>
       <c r="P18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="Q18" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="U18" t="s">
         <v>36</v>
@@ -1842,10 +1846,10 @@
         <v>92</v>
       </c>
       <c r="P19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="Q19" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="U19" t="s">
         <v>36</v>
@@ -1898,10 +1902,10 @@
         <v>76</v>
       </c>
       <c r="P20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="Q20" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="U20" t="s">
         <v>49</v>
@@ -1954,10 +1958,10 @@
         <v>88</v>
       </c>
       <c r="P21" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="Q21" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="U21" t="s">
         <v>36</v>
@@ -2010,10 +2014,10 @@
         <v>35</v>
       </c>
       <c r="P22" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q22" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="U22" t="s">
         <v>36</v>
@@ -2066,10 +2070,10 @@
         <v>65</v>
       </c>
       <c r="P23" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q23" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="U23" t="s">
         <v>36</v>
@@ -2122,10 +2126,10 @@
         <v>58</v>
       </c>
       <c r="P24" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q24" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="U24" t="s">
         <v>49</v>
@@ -2178,10 +2182,10 @@
         <v>69</v>
       </c>
       <c r="P25" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q25" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="U25" t="s">
         <v>36</v>
@@ -2234,10 +2238,10 @@
         <v>48</v>
       </c>
       <c r="P26" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q26" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="U26" t="s">
         <v>49</v>

</xml_diff>